<commit_message>
fix sch pin error pa2-->pa5
</commit_message>
<xml_diff>
--- a/HARDWARE/DOC/pin分配.xlsx
+++ b/HARDWARE/DOC/pin分配.xlsx
@@ -62,10 +62,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PA2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PA4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -99,6 +95,10 @@
   </si>
   <si>
     <t>PA10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -478,7 +478,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -508,7 +508,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>4</v>
@@ -522,13 +522,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="4" customFormat="1">
@@ -536,7 +536,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>4</v>
@@ -550,13 +550,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="4" customFormat="1">
@@ -564,7 +564,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>7</v>
@@ -578,7 +578,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>8</v>

</xml_diff>